<commit_message>
Updated excess mortality main function to use new bg population function.
Signed-off-by: Mlad-en <mmladenov1992@gmail.com>
</commit_message>
<xml_diff>
--- a/data_output/Excess Mortality/Countries/TOTAL_EUROPE_(0-4) - (70-74)_['Female', 'Male', 'Total']_excess_mortality_2020.xlsx
+++ b/data_output/Excess Mortality/Countries/TOTAL_EUROPE_(0-4) - (70-74)_['Female', 'Male', 'Total']_excess_mortality_2020.xlsx
@@ -662,7 +662,7 @@
         <v>2020</v>
       </c>
       <c r="D3" t="n">
-        <v>11760</v>
+        <v>11767</v>
       </c>
       <c r="E3" t="n">
         <v>10679</v>
@@ -698,7 +698,7 @@
         <v>10873.4</v>
       </c>
       <c r="P3" t="n">
-        <v>1037</v>
+        <v>1044</v>
       </c>
       <c r="Q3" t="n">
         <v>150.4</v>
@@ -716,7 +716,7 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>1037.0 (±150.4)</t>
+          <t>1044.0 (±150.4)</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
@@ -728,14 +728,14 @@
         <v>5220663</v>
       </c>
       <c r="X3" t="n">
-        <v>19.9</v>
+        <v>20</v>
       </c>
       <c r="Y3" t="n">
-        <v>2.8</v>
+        <v>2.9</v>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>19.9(±2.8)</t>
+          <t>20.0(±2.9)</t>
         </is>
       </c>
     </row>
@@ -846,7 +846,7 @@
         <v>2020</v>
       </c>
       <c r="D5" t="n">
-        <v>5782</v>
+        <v>5773</v>
       </c>
       <c r="E5" t="n">
         <v>5502</v>
@@ -882,16 +882,16 @@
         <v>5412.900000000001</v>
       </c>
       <c r="P5" t="n">
-        <v>543.8</v>
+        <v>534.8</v>
       </c>
       <c r="Q5" t="n">
         <v>174.7</v>
       </c>
       <c r="R5" t="n">
-        <v>10.4</v>
+        <v>10.2</v>
       </c>
       <c r="S5" t="n">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="T5" t="inlineStr">
         <is>
@@ -900,26 +900,26 @@
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>543.8 (±174.7)</t>
+          <t>534.8 (±174.7)</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>10.4% (±3.6%)</t>
+          <t>10.2% (±3.5%)</t>
         </is>
       </c>
       <c r="W5" t="n">
         <v>1840571</v>
       </c>
       <c r="X5" t="n">
-        <v>29.5</v>
+        <v>29.1</v>
       </c>
       <c r="Y5" t="n">
-        <v>9.5</v>
+        <v>9.4</v>
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>29.5(±9.5)</t>
+          <t>29.1(±9.4)</t>
         </is>
       </c>
     </row>
@@ -1214,7 +1214,7 @@
         <v>2020</v>
       </c>
       <c r="D9" t="n">
-        <v>1743</v>
+        <v>1744</v>
       </c>
       <c r="E9" t="n">
         <v>1644</v>
@@ -1250,7 +1250,7 @@
         <v>1644.3</v>
       </c>
       <c r="P9" t="n">
-        <v>144.8</v>
+        <v>145.8</v>
       </c>
       <c r="Q9" t="n">
         <v>46.1</v>
@@ -1259,7 +1259,7 @@
         <v>9.1</v>
       </c>
       <c r="S9" t="n">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="T9" t="inlineStr">
         <is>
@@ -1268,26 +1268,26 @@
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>144.8 (±46.1)</t>
+          <t>145.8 (±46.1)</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>9.1% (±3.1%)</t>
+          <t>9.1% (±3.0%)</t>
         </is>
       </c>
       <c r="W9" t="n">
         <v>610017</v>
       </c>
       <c r="X9" t="n">
-        <v>23.7</v>
+        <v>23.9</v>
       </c>
       <c r="Y9" t="n">
         <v>7.6</v>
       </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>23.7(±7.6)</t>
+          <t>23.9(±7.6)</t>
         </is>
       </c>
     </row>
@@ -1398,7 +1398,7 @@
         <v>2020</v>
       </c>
       <c r="D11" t="n">
-        <v>58305</v>
+        <v>58317</v>
       </c>
       <c r="E11" t="n">
         <v>51209</v>
@@ -1434,13 +1434,13 @@
         <v>54266.6</v>
       </c>
       <c r="P11" t="n">
-        <v>4788</v>
+        <v>4800</v>
       </c>
       <c r="Q11" t="n">
         <v>749.6</v>
       </c>
       <c r="R11" t="n">
-        <v>8.9</v>
+        <v>9</v>
       </c>
       <c r="S11" t="n">
         <v>1.5</v>
@@ -1452,12 +1452,12 @@
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>4788.0 (±749.6)</t>
+          <t>4800.0 (±749.6)</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>8.9% (±1.5%)</t>
+          <t>9.0% (±1.5%)</t>
         </is>
       </c>
       <c r="W11" t="n">
@@ -1467,11 +1467,11 @@
         <v>15.5</v>
       </c>
       <c r="Y11" t="n">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>15.5(±2.4)</t>
+          <t>15.5(±2.5)</t>
         </is>
       </c>
     </row>
@@ -1766,7 +1766,7 @@
         <v>2020</v>
       </c>
       <c r="D15" t="n">
-        <v>54353</v>
+        <v>54369</v>
       </c>
       <c r="E15" t="n">
         <v>50149</v>
@@ -1802,7 +1802,7 @@
         <v>50033.6</v>
       </c>
       <c r="P15" t="n">
-        <v>5389</v>
+        <v>5405</v>
       </c>
       <c r="Q15" t="n">
         <v>1069.6</v>
@@ -1811,7 +1811,7 @@
         <v>11</v>
       </c>
       <c r="S15" t="n">
-        <v>2.4</v>
+        <v>2.3</v>
       </c>
       <c r="T15" t="inlineStr">
         <is>
@@ -1820,26 +1820,26 @@
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>5389.0 (±1069.6)</t>
+          <t>5405.0 (±1069.6)</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>11.0% (±2.4%)</t>
+          <t>11.0% (±2.3%)</t>
         </is>
       </c>
       <c r="W15" t="n">
         <v>26364108</v>
       </c>
       <c r="X15" t="n">
-        <v>20.4</v>
+        <v>20.5</v>
       </c>
       <c r="Y15" t="n">
         <v>4.1</v>
       </c>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>20.4(±4.1)</t>
+          <t>20.5(±4.1)</t>
         </is>
       </c>
     </row>
@@ -1950,7 +1950,7 @@
         <v>2020</v>
       </c>
       <c r="D17" t="n">
-        <v>4926</v>
+        <v>5003</v>
       </c>
       <c r="E17" t="n">
         <v>4845</v>
@@ -1986,16 +1986,16 @@
         <v>4747.9</v>
       </c>
       <c r="P17" t="n">
-        <v>413.2</v>
+        <v>490.2</v>
       </c>
       <c r="Q17" t="n">
         <v>235.1</v>
       </c>
       <c r="R17" t="n">
-        <v>9.199999999999999</v>
+        <v>10.9</v>
       </c>
       <c r="S17" t="n">
-        <v>5.4</v>
+        <v>5.5</v>
       </c>
       <c r="T17" t="inlineStr">
         <is>
@@ -2004,26 +2004,26 @@
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>413.2 (±235.1)</t>
+          <t>490.2 (±235.1)</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>9.2% (±5.4%)</t>
+          <t>10.9% (±5.5%)</t>
         </is>
       </c>
       <c r="W17" t="n">
         <v>1294861</v>
       </c>
       <c r="X17" t="n">
-        <v>31.9</v>
+        <v>37.9</v>
       </c>
       <c r="Y17" t="n">
-        <v>18.2</v>
+        <v>18.1</v>
       </c>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>31.9(±18.2)</t>
+          <t>37.9(±18.1)</t>
         </is>
       </c>
     </row>
@@ -2042,7 +2042,7 @@
         <v>2020</v>
       </c>
       <c r="D18" t="n">
-        <v>469</v>
+        <v>450</v>
       </c>
       <c r="E18" t="n">
         <v>401</v>
@@ -2078,16 +2078,16 @@
         <v>440.0000000000001</v>
       </c>
       <c r="P18" t="n">
-        <v>46.4</v>
+        <v>27.4</v>
       </c>
       <c r="Q18" t="n">
         <v>17.4</v>
       </c>
       <c r="R18" t="n">
-        <v>11</v>
+        <v>6.5</v>
       </c>
       <c r="S18" t="n">
-        <v>4.4</v>
+        <v>4.2</v>
       </c>
       <c r="T18" t="inlineStr">
         <is>
@@ -2096,26 +2096,26 @@
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>46.4 (±17.4)</t>
+          <t>27.4 (±17.4)</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>11.0% (±4.4%)</t>
+          <t>6.5% (±4.2%)</t>
         </is>
       </c>
       <c r="W18" t="n">
         <v>286685</v>
       </c>
       <c r="X18" t="n">
-        <v>16.2</v>
+        <v>9.6</v>
       </c>
       <c r="Y18" t="n">
-        <v>6.1</v>
+        <v>6</v>
       </c>
       <c r="Z18" t="inlineStr">
         <is>
-          <t>16.2(±6.1)</t>
+          <t>9.6(±6.0)</t>
         </is>
       </c>
     </row>
@@ -2226,7 +2226,7 @@
         <v>2020</v>
       </c>
       <c r="D20" t="n">
-        <v>999</v>
+        <v>1010</v>
       </c>
       <c r="E20" t="n">
         <v>891</v>
@@ -2262,16 +2262,16 @@
         <v>896.5999999999999</v>
       </c>
       <c r="P20" t="n">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="Q20" t="n">
         <v>32.6</v>
       </c>
       <c r="R20" t="n">
-        <v>15.6</v>
+        <v>16.9</v>
       </c>
       <c r="S20" t="n">
-        <v>4.2</v>
+        <v>4.3</v>
       </c>
       <c r="T20" t="inlineStr">
         <is>
@@ -2280,26 +2280,26 @@
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>135.0 (±32.6)</t>
+          <t>146.0 (±32.6)</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>15.6% (±4.2%)</t>
+          <t>16.9% (±4.3%)</t>
         </is>
       </c>
       <c r="W20" t="n">
         <v>292082</v>
       </c>
       <c r="X20" t="n">
-        <v>46.2</v>
+        <v>50</v>
       </c>
       <c r="Y20" t="n">
-        <v>11.2</v>
+        <v>11.1</v>
       </c>
       <c r="Z20" t="inlineStr">
         <is>
-          <t>46.2(±11.2)</t>
+          <t>50.0(±11.1)</t>
         </is>
       </c>
     </row>
@@ -2410,7 +2410,7 @@
         <v>2020</v>
       </c>
       <c r="D22" t="n">
-        <v>4085</v>
+        <v>4086</v>
       </c>
       <c r="E22" t="n">
         <v>4054</v>
@@ -2446,7 +2446,7 @@
         <v>4163.099999999999</v>
       </c>
       <c r="P22" t="n">
-        <v>-50.8</v>
+        <v>-49.8</v>
       </c>
       <c r="Q22" t="n">
         <v>27.3</v>
@@ -2464,7 +2464,7 @@
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>-50.8 (±27.3)</t>
+          <t>-49.8 (±27.3)</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
@@ -2479,11 +2479,11 @@
         <v>-2.1</v>
       </c>
       <c r="Y22" t="n">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
       <c r="Z22" t="inlineStr">
         <is>
-          <t>-2.1(±1.1)</t>
+          <t>-2.1(±1.2)</t>
         </is>
       </c>
     </row>
@@ -2594,7 +2594,7 @@
         <v>2020</v>
       </c>
       <c r="D24" t="n">
-        <v>9741</v>
+        <v>9775</v>
       </c>
       <c r="E24" t="n">
         <v>8684</v>
@@ -2630,13 +2630,13 @@
         <v>9085.799999999999</v>
       </c>
       <c r="P24" t="n">
-        <v>746.4</v>
+        <v>780.4</v>
       </c>
       <c r="Q24" t="n">
         <v>91.2</v>
       </c>
       <c r="R24" t="n">
-        <v>8.300000000000001</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="S24" t="n">
         <v>1.1</v>
@@ -2648,26 +2648,26 @@
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>746.4 (±91.2)</t>
+          <t>780.4 (±91.2)</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>8.3% (±1.1%)</t>
+          <t>8.7% (±1.1%)</t>
         </is>
       </c>
       <c r="W24" t="n">
         <v>4752501</v>
       </c>
       <c r="X24" t="n">
-        <v>15.7</v>
+        <v>16.4</v>
       </c>
       <c r="Y24" t="n">
         <v>1.9</v>
       </c>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>15.7(±1.9)</t>
+          <t>16.4(±1.9)</t>
         </is>
       </c>
     </row>
@@ -2778,7 +2778,7 @@
         <v>2020</v>
       </c>
       <c r="D26" t="n">
-        <v>8016</v>
+        <v>8017</v>
       </c>
       <c r="E26" t="n">
         <v>7100</v>
@@ -2814,7 +2814,7 @@
         <v>7229.899999999999</v>
       </c>
       <c r="P26" t="n">
-        <v>872.4</v>
+        <v>873.4</v>
       </c>
       <c r="Q26" t="n">
         <v>86.3</v>
@@ -2832,7 +2832,7 @@
       </c>
       <c r="U26" t="inlineStr">
         <is>
-          <t>872.4 (±86.3)</t>
+          <t>873.4 (±86.3)</t>
         </is>
       </c>
       <c r="V26" t="inlineStr">
@@ -2844,14 +2844,14 @@
         <v>2564041</v>
       </c>
       <c r="X26" t="n">
-        <v>34</v>
+        <v>34.1</v>
       </c>
       <c r="Y26" t="n">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>34.0(±3.4)</t>
+          <t>34.1(±3.3)</t>
         </is>
       </c>
     </row>
@@ -3146,7 +3146,7 @@
         <v>2020</v>
       </c>
       <c r="D30" t="n">
-        <v>5869</v>
+        <v>5877</v>
       </c>
       <c r="E30" t="n">
         <v>5835</v>
@@ -3182,13 +3182,13 @@
         <v>5880.499999999998</v>
       </c>
       <c r="P30" t="n">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="Q30" t="n">
         <v>79.5</v>
       </c>
       <c r="R30" t="n">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="S30" t="n">
         <v>1.4</v>
@@ -3200,26 +3200,26 @@
       </c>
       <c r="U30" t="inlineStr">
         <is>
-          <t>68.0 (±79.5)</t>
+          <t>76.0 (±79.5)</t>
         </is>
       </c>
       <c r="V30" t="inlineStr">
         <is>
-          <t>1.2% (±1.4%)</t>
+          <t>1.3% (±1.4%)</t>
         </is>
       </c>
       <c r="W30" t="n">
         <v>3882539</v>
       </c>
       <c r="X30" t="n">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="Y30" t="n">
         <v>2</v>
       </c>
       <c r="Z30" t="inlineStr">
         <is>
-          <t>1.8(±2.0)</t>
+          <t>2.0(±2.0)</t>
         </is>
       </c>
     </row>
@@ -3330,7 +3330,7 @@
         <v>2020</v>
       </c>
       <c r="D32" t="n">
-        <v>19838</v>
+        <v>19847</v>
       </c>
       <c r="E32" t="n">
         <v>17569</v>
@@ -3366,16 +3366,16 @@
         <v>17781.1</v>
       </c>
       <c r="P32" t="n">
-        <v>2253.2</v>
+        <v>2262.2</v>
       </c>
       <c r="Q32" t="n">
         <v>196.3</v>
       </c>
       <c r="R32" t="n">
-        <v>12.8</v>
+        <v>12.9</v>
       </c>
       <c r="S32" t="n">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="T32" t="inlineStr">
         <is>
@@ -3384,26 +3384,26 @@
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>2253.2 (±196.3)</t>
+          <t>2262.2 (±196.3)</t>
         </is>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>12.8% (±1.2%)</t>
+          <t>12.9% (±1.3%)</t>
         </is>
       </c>
       <c r="W32" t="n">
         <v>5267710</v>
       </c>
       <c r="X32" t="n">
-        <v>42.8</v>
+        <v>42.9</v>
       </c>
       <c r="Y32" t="n">
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
       <c r="Z32" t="inlineStr">
         <is>
-          <t>42.8(±3.7)</t>
+          <t>42.9(±3.8)</t>
         </is>
       </c>
     </row>
@@ -3422,7 +3422,7 @@
         <v>2020</v>
       </c>
       <c r="D33" t="n">
-        <v>31006</v>
+        <v>31009</v>
       </c>
       <c r="E33" t="n">
         <v>25361</v>
@@ -3458,16 +3458,16 @@
         <v>25584.2</v>
       </c>
       <c r="P33" t="n">
-        <v>5765.4</v>
+        <v>5768.4</v>
       </c>
       <c r="Q33" t="n">
         <v>343.6</v>
       </c>
       <c r="R33" t="n">
-        <v>22.8</v>
+        <v>22.9</v>
       </c>
       <c r="S33" t="n">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="T33" t="inlineStr">
         <is>
@@ -3476,26 +3476,26 @@
       </c>
       <c r="U33" t="inlineStr">
         <is>
-          <t>5765.4 (±343.6)</t>
+          <t>5768.4 (±343.6)</t>
         </is>
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>22.8% (±1.6%)</t>
+          <t>22.9% (±1.7%)</t>
         </is>
       </c>
       <c r="W33" t="n">
         <v>3143603</v>
       </c>
       <c r="X33" t="n">
-        <v>183.4</v>
+        <v>183.5</v>
       </c>
       <c r="Y33" t="n">
         <v>10.9</v>
       </c>
       <c r="Z33" t="inlineStr">
         <is>
-          <t>183.4(±10.9)</t>
+          <t>183.5(±10.9)</t>
         </is>
       </c>
     </row>
@@ -3514,7 +3514,7 @@
         <v>2020</v>
       </c>
       <c r="D34" t="n">
-        <v>11445</v>
+        <v>11426</v>
       </c>
       <c r="E34" t="n">
         <v>10539</v>
@@ -3550,16 +3550,16 @@
         <v>10537.5</v>
       </c>
       <c r="P34" t="n">
-        <v>1147.8</v>
+        <v>1128.8</v>
       </c>
       <c r="Q34" t="n">
         <v>240.3</v>
       </c>
       <c r="R34" t="n">
-        <v>11.1</v>
+        <v>11</v>
       </c>
       <c r="S34" t="n">
-        <v>2.5</v>
+        <v>2.6</v>
       </c>
       <c r="T34" t="inlineStr">
         <is>
@@ -3568,26 +3568,26 @@
       </c>
       <c r="U34" t="inlineStr">
         <is>
-          <t>1147.8 (±240.3)</t>
+          <t>1128.8 (±240.3)</t>
         </is>
       </c>
       <c r="V34" t="inlineStr">
         <is>
-          <t>11.1% (±2.5%)</t>
+          <t>11.0% (±2.6%)</t>
         </is>
       </c>
       <c r="W34" t="n">
         <v>1834316</v>
       </c>
       <c r="X34" t="n">
-        <v>62.6</v>
+        <v>61.5</v>
       </c>
       <c r="Y34" t="n">
         <v>13.1</v>
       </c>
       <c r="Z34" t="inlineStr">
         <is>
-          <t>62.6(±13.1)</t>
+          <t>61.5(±13.1)</t>
         </is>
       </c>
     </row>
@@ -3698,7 +3698,7 @@
         <v>2020</v>
       </c>
       <c r="D36" t="n">
-        <v>27889</v>
+        <v>27890</v>
       </c>
       <c r="E36" t="n">
         <v>24878</v>
@@ -3734,7 +3734,7 @@
         <v>25057.5</v>
       </c>
       <c r="P36" t="n">
-        <v>3141.4</v>
+        <v>3142.4</v>
       </c>
       <c r="Q36" t="n">
         <v>309.9</v>
@@ -3752,7 +3752,7 @@
       </c>
       <c r="U36" t="inlineStr">
         <is>
-          <t>3141.4 (±309.9)</t>
+          <t>3142.4 (±309.9)</t>
         </is>
       </c>
       <c r="V36" t="inlineStr">
@@ -3767,11 +3767,11 @@
         <v>63.4</v>
       </c>
       <c r="Y36" t="n">
-        <v>6.2</v>
+        <v>6.3</v>
       </c>
       <c r="Z36" t="inlineStr">
         <is>
-          <t>63.4(±6.2)</t>
+          <t>63.4(±6.3)</t>
         </is>
       </c>
     </row>
@@ -3882,7 +3882,7 @@
         <v>2020</v>
       </c>
       <c r="D38" t="n">
-        <v>3500</v>
+        <v>3501</v>
       </c>
       <c r="E38" t="n">
         <v>3415</v>
@@ -3918,7 +3918,7 @@
         <v>3414.2</v>
       </c>
       <c r="P38" t="n">
-        <v>160.4</v>
+        <v>161.4</v>
       </c>
       <c r="Q38" t="n">
         <v>74.59999999999999</v>
@@ -3936,7 +3936,7 @@
       </c>
       <c r="U38" t="inlineStr">
         <is>
-          <t>160.4 (±74.6)</t>
+          <t>161.4 (±74.6)</t>
         </is>
       </c>
       <c r="V38" t="inlineStr">
@@ -3948,14 +3948,14 @@
         <v>592881</v>
       </c>
       <c r="X38" t="n">
-        <v>27.1</v>
+        <v>27.2</v>
       </c>
       <c r="Y38" t="n">
-        <v>12.5</v>
+        <v>12.6</v>
       </c>
       <c r="Z38" t="inlineStr">
         <is>
-          <t>27.1(±12.5)</t>
+          <t>27.2(±12.6)</t>
         </is>
       </c>
     </row>
@@ -3974,7 +3974,7 @@
         <v>2020</v>
       </c>
       <c r="D39" t="n">
-        <v>9940</v>
+        <v>9941</v>
       </c>
       <c r="E39" t="n">
         <v>9766</v>
@@ -4010,7 +4010,7 @@
         <v>9895.000000000002</v>
       </c>
       <c r="P39" t="n">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="Q39" t="n">
         <v>103</v>
@@ -4028,7 +4028,7 @@
       </c>
       <c r="U39" t="inlineStr">
         <is>
-          <t>148.0 (±103.0)</t>
+          <t>149.0 (±103.0)</t>
         </is>
       </c>
       <c r="V39" t="inlineStr">
@@ -4066,7 +4066,7 @@
         <v>2020</v>
       </c>
       <c r="D40" t="n">
-        <v>109687</v>
+        <v>109718</v>
       </c>
       <c r="E40" t="n">
         <v>100799</v>
@@ -4102,16 +4102,16 @@
         <v>102232.7</v>
       </c>
       <c r="P40" t="n">
-        <v>7983</v>
+        <v>8014</v>
       </c>
       <c r="Q40" t="n">
         <v>528.7</v>
       </c>
       <c r="R40" t="n">
-        <v>7.8</v>
+        <v>7.9</v>
       </c>
       <c r="S40" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="T40" t="inlineStr">
         <is>
@@ -4120,26 +4120,26 @@
       </c>
       <c r="U40" t="inlineStr">
         <is>
-          <t>7983.0 (±528.7)</t>
+          <t>8014.0 (±528.7)</t>
         </is>
       </c>
       <c r="V40" t="inlineStr">
         <is>
-          <t>7.8% (±0.5%)</t>
+          <t>7.9% (±0.6%)</t>
         </is>
       </c>
       <c r="W40" t="n">
         <v>30056581</v>
       </c>
       <c r="X40" t="n">
-        <v>26.6</v>
+        <v>26.7</v>
       </c>
       <c r="Y40" t="n">
         <v>1.7</v>
       </c>
       <c r="Z40" t="inlineStr">
         <is>
-          <t>26.6(±1.7)</t>
+          <t>26.7(±1.7)</t>
         </is>
       </c>
     </row>
@@ -4434,7 +4434,7 @@
         <v>2020</v>
       </c>
       <c r="D44" t="n">
-        <v>95194</v>
+        <v>95200</v>
       </c>
       <c r="E44" t="n">
         <v>83640</v>
@@ -4470,7 +4470,7 @@
         <v>83155.10000000001</v>
       </c>
       <c r="P44" t="n">
-        <v>14194.2</v>
+        <v>14200.2</v>
       </c>
       <c r="Q44" t="n">
         <v>2155.3</v>
@@ -4488,7 +4488,7 @@
       </c>
       <c r="U44" t="inlineStr">
         <is>
-          <t>14194.2 (±2155.3)</t>
+          <t>14200.2 (±2155.3)</t>
         </is>
       </c>
       <c r="V44" t="inlineStr">
@@ -4500,14 +4500,14 @@
         <v>26213664</v>
       </c>
       <c r="X44" t="n">
-        <v>54.1</v>
+        <v>54.2</v>
       </c>
       <c r="Y44" t="n">
-        <v>8.300000000000001</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="Z44" t="inlineStr">
         <is>
-          <t>54.1(±8.3)</t>
+          <t>54.2(±8.2)</t>
         </is>
       </c>
     </row>
@@ -4618,7 +4618,7 @@
         <v>2020</v>
       </c>
       <c r="D46" t="n">
-        <v>10249</v>
+        <v>10460</v>
       </c>
       <c r="E46" t="n">
         <v>10297</v>
@@ -4654,16 +4654,16 @@
         <v>9983.600000000002</v>
       </c>
       <c r="P46" t="n">
-        <v>904.6</v>
+        <v>1115.6</v>
       </c>
       <c r="Q46" t="n">
         <v>639.2</v>
       </c>
       <c r="R46" t="n">
-        <v>9.699999999999999</v>
+        <v>11.9</v>
       </c>
       <c r="S46" t="n">
-        <v>7</v>
+        <v>7.1</v>
       </c>
       <c r="T46" t="inlineStr">
         <is>
@@ -4672,26 +4672,26 @@
       </c>
       <c r="U46" t="inlineStr">
         <is>
-          <t>904.6 (±639.2)</t>
+          <t>1115.6 (±639.2)</t>
         </is>
       </c>
       <c r="V46" t="inlineStr">
         <is>
-          <t>9.7% (±7.0%)</t>
+          <t>11.9% (±7.1%)</t>
         </is>
       </c>
       <c r="W46" t="n">
         <v>1224273</v>
       </c>
       <c r="X46" t="n">
-        <v>73.90000000000001</v>
+        <v>91.09999999999999</v>
       </c>
       <c r="Y46" t="n">
         <v>52.2</v>
       </c>
       <c r="Z46" t="inlineStr">
         <is>
-          <t>73.9(±52.2)</t>
+          <t>91.1(±52.2)</t>
         </is>
       </c>
     </row>
@@ -4710,7 +4710,7 @@
         <v>2020</v>
       </c>
       <c r="D47" t="n">
-        <v>857</v>
+        <v>842</v>
       </c>
       <c r="E47" t="n">
         <v>688</v>
@@ -4746,16 +4746,16 @@
         <v>786.6999999999998</v>
       </c>
       <c r="P47" t="n">
-        <v>99.8</v>
+        <v>84.8</v>
       </c>
       <c r="Q47" t="n">
         <v>29.5</v>
       </c>
       <c r="R47" t="n">
-        <v>13.2</v>
+        <v>11.2</v>
       </c>
       <c r="S47" t="n">
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="T47" t="inlineStr">
         <is>
@@ -4764,26 +4764,26 @@
       </c>
       <c r="U47" t="inlineStr">
         <is>
-          <t>99.8 (±29.5)</t>
+          <t>84.8 (±29.5)</t>
         </is>
       </c>
       <c r="V47" t="inlineStr">
         <is>
-          <t>13.2% (±4.3%)</t>
+          <t>11.2% (±4.2%)</t>
         </is>
       </c>
       <c r="W47" t="n">
         <v>298206</v>
       </c>
       <c r="X47" t="n">
-        <v>33.5</v>
+        <v>28.4</v>
       </c>
       <c r="Y47" t="n">
         <v>9.9</v>
       </c>
       <c r="Z47" t="inlineStr">
         <is>
-          <t>33.5(±9.9)</t>
+          <t>28.4(±9.9)</t>
         </is>
       </c>
     </row>
@@ -4894,7 +4894,7 @@
         <v>2020</v>
       </c>
       <c r="D49" t="n">
-        <v>1769</v>
+        <v>1789</v>
       </c>
       <c r="E49" t="n">
         <v>1393</v>
@@ -4930,16 +4930,16 @@
         <v>1512</v>
       </c>
       <c r="P49" t="n">
-        <v>297.4</v>
+        <v>317.4</v>
       </c>
       <c r="Q49" t="n">
         <v>40.4</v>
       </c>
       <c r="R49" t="n">
-        <v>20.2</v>
+        <v>21.6</v>
       </c>
       <c r="S49" t="n">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="T49" t="inlineStr">
         <is>
@@ -4948,26 +4948,26 @@
       </c>
       <c r="U49" t="inlineStr">
         <is>
-          <t>297.4 (±40.4)</t>
+          <t>317.4 (±40.4)</t>
         </is>
       </c>
       <c r="V49" t="inlineStr">
         <is>
-          <t>20.2% (±3.2%)</t>
+          <t>21.6% (±3.3%)</t>
         </is>
       </c>
       <c r="W49" t="n">
         <v>292748</v>
       </c>
       <c r="X49" t="n">
-        <v>101.6</v>
+        <v>108.4</v>
       </c>
       <c r="Y49" t="n">
         <v>13.8</v>
       </c>
       <c r="Z49" t="inlineStr">
         <is>
-          <t>101.6(±13.8)</t>
+          <t>108.4(±13.8)</t>
         </is>
       </c>
     </row>
@@ -5262,7 +5262,7 @@
         <v>2020</v>
       </c>
       <c r="D53" t="n">
-        <v>19193</v>
+        <v>19265</v>
       </c>
       <c r="E53" t="n">
         <v>17158</v>
@@ -5298,16 +5298,16 @@
         <v>17729.3</v>
       </c>
       <c r="P53" t="n">
-        <v>1591.8</v>
+        <v>1663.8</v>
       </c>
       <c r="Q53" t="n">
         <v>128.1</v>
       </c>
       <c r="R53" t="n">
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="S53" t="n">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="T53" t="inlineStr">
         <is>
@@ -5316,26 +5316,26 @@
       </c>
       <c r="U53" t="inlineStr">
         <is>
-          <t>1591.8 (±128.1)</t>
+          <t>1663.8 (±128.1)</t>
         </is>
       </c>
       <c r="V53" t="inlineStr">
         <is>
-          <t>9.0% (±0.7%)</t>
+          <t>9.5% (±0.8%)</t>
         </is>
       </c>
       <c r="W53" t="n">
         <v>4435487</v>
       </c>
       <c r="X53" t="n">
-        <v>35.9</v>
+        <v>37.5</v>
       </c>
       <c r="Y53" t="n">
         <v>2.9</v>
       </c>
       <c r="Z53" t="inlineStr">
         <is>
-          <t>35.9(±2.9)</t>
+          <t>37.5(±2.9)</t>
         </is>
       </c>
     </row>
@@ -5446,7 +5446,7 @@
         <v>2020</v>
       </c>
       <c r="D55" t="n">
-        <v>15294</v>
+        <v>15286</v>
       </c>
       <c r="E55" t="n">
         <v>13836</v>
@@ -5482,13 +5482,13 @@
         <v>13966.8</v>
       </c>
       <c r="P55" t="n">
-        <v>1489.8</v>
+        <v>1481.8</v>
       </c>
       <c r="Q55" t="n">
         <v>162.6</v>
       </c>
       <c r="R55" t="n">
-        <v>10.8</v>
+        <v>10.7</v>
       </c>
       <c r="S55" t="n">
         <v>1.3</v>
@@ -5500,26 +5500,26 @@
       </c>
       <c r="U55" t="inlineStr">
         <is>
-          <t>1489.8 (±162.6)</t>
+          <t>1481.8 (±162.6)</t>
         </is>
       </c>
       <c r="V55" t="inlineStr">
         <is>
-          <t>10.8% (±1.3%)</t>
+          <t>10.7% (±1.3%)</t>
         </is>
       </c>
       <c r="W55" t="n">
         <v>2549303</v>
       </c>
       <c r="X55" t="n">
-        <v>58.4</v>
+        <v>58.1</v>
       </c>
       <c r="Y55" t="n">
         <v>6.4</v>
       </c>
       <c r="Z55" t="inlineStr">
         <is>
-          <t>58.4(±6.4)</t>
+          <t>58.1(±6.4)</t>
         </is>
       </c>
     </row>
@@ -5630,7 +5630,7 @@
         <v>2020</v>
       </c>
       <c r="D57" t="n">
-        <v>73171</v>
+        <v>73174</v>
       </c>
       <c r="E57" t="n">
         <v>62634</v>
@@ -5666,7 +5666,7 @@
         <v>63420.99999999999</v>
       </c>
       <c r="P57" t="n">
-        <v>10180</v>
+        <v>10183</v>
       </c>
       <c r="Q57" t="n">
         <v>430</v>
@@ -5684,7 +5684,7 @@
       </c>
       <c r="U57" t="inlineStr">
         <is>
-          <t>10180.0 (±430.0)</t>
+          <t>10183.0 (±430.0)</t>
         </is>
       </c>
       <c r="V57" t="inlineStr">
@@ -5814,7 +5814,7 @@
         <v>2020</v>
       </c>
       <c r="D59" t="n">
-        <v>9962</v>
+        <v>9982</v>
       </c>
       <c r="E59" t="n">
         <v>9802</v>
@@ -5850,13 +5850,13 @@
         <v>9717.899999999998</v>
       </c>
       <c r="P59" t="n">
-        <v>471.6</v>
+        <v>491.6</v>
       </c>
       <c r="Q59" t="n">
         <v>227.5</v>
       </c>
       <c r="R59" t="n">
-        <v>5</v>
+        <v>5.2</v>
       </c>
       <c r="S59" t="n">
         <v>2.5</v>
@@ -5868,26 +5868,26 @@
       </c>
       <c r="U59" t="inlineStr">
         <is>
-          <t>471.6 (±227.5)</t>
+          <t>491.6 (±227.5)</t>
         </is>
       </c>
       <c r="V59" t="inlineStr">
         <is>
-          <t>5.0% (±2.5%)</t>
+          <t>5.2% (±2.5%)</t>
         </is>
       </c>
       <c r="W59" t="n">
         <v>3948397</v>
       </c>
       <c r="X59" t="n">
-        <v>11.9</v>
+        <v>12.5</v>
       </c>
       <c r="Y59" t="n">
-        <v>5.8</v>
+        <v>5.7</v>
       </c>
       <c r="Z59" t="inlineStr">
         <is>
-          <t>11.9(±5.8)</t>
+          <t>12.5(±5.7)</t>
         </is>
       </c>
     </row>
@@ -5998,7 +5998,7 @@
         <v>2020</v>
       </c>
       <c r="D61" t="n">
-        <v>31598</v>
+        <v>31614</v>
       </c>
       <c r="E61" t="n">
         <v>28248</v>
@@ -6034,13 +6034,13 @@
         <v>28542.3</v>
       </c>
       <c r="P61" t="n">
-        <v>3290.2</v>
+        <v>3306.2</v>
       </c>
       <c r="Q61" t="n">
         <v>234.5</v>
       </c>
       <c r="R61" t="n">
-        <v>11.6</v>
+        <v>11.7</v>
       </c>
       <c r="S61" t="n">
         <v>0.9</v>
@@ -6052,26 +6052,26 @@
       </c>
       <c r="U61" t="inlineStr">
         <is>
-          <t>3290.2 (±234.5)</t>
+          <t>3306.2 (±234.5)</t>
         </is>
       </c>
       <c r="V61" t="inlineStr">
         <is>
-          <t>11.6% (±0.9%)</t>
+          <t>11.7% (±0.9%)</t>
         </is>
       </c>
       <c r="W61" t="n">
         <v>10488373</v>
       </c>
       <c r="X61" t="n">
-        <v>31.4</v>
+        <v>31.5</v>
       </c>
       <c r="Y61" t="n">
-        <v>2.2</v>
+        <v>2.3</v>
       </c>
       <c r="Z61" t="inlineStr">
         <is>
-          <t>31.4(±2.2)</t>
+          <t>31.5(±2.3)</t>
         </is>
       </c>
     </row>
@@ -6090,7 +6090,7 @@
         <v>2020</v>
       </c>
       <c r="D62" t="n">
-        <v>47909</v>
+        <v>47912</v>
       </c>
       <c r="E62" t="n">
         <v>38984</v>
@@ -6126,7 +6126,7 @@
         <v>39286.69999999999</v>
       </c>
       <c r="P62" t="n">
-        <v>9123</v>
+        <v>9126</v>
       </c>
       <c r="Q62" t="n">
         <v>500.7</v>
@@ -6135,7 +6135,7 @@
         <v>23.5</v>
       </c>
       <c r="S62" t="n">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="T62" t="inlineStr">
         <is>
@@ -6144,26 +6144,26 @@
       </c>
       <c r="U62" t="inlineStr">
         <is>
-          <t>9123.0 (±500.7)</t>
+          <t>9126.0 (±500.7)</t>
         </is>
       </c>
       <c r="V62" t="inlineStr">
         <is>
-          <t>23.5% (±1.6%)</t>
+          <t>23.5% (±1.5%)</t>
         </is>
       </c>
       <c r="W62" t="n">
         <v>6329301</v>
       </c>
       <c r="X62" t="n">
-        <v>144.1</v>
+        <v>144.2</v>
       </c>
       <c r="Y62" t="n">
         <v>7.9</v>
       </c>
       <c r="Z62" t="inlineStr">
         <is>
-          <t>144.1(±7.9)</t>
+          <t>144.2(±7.9)</t>
         </is>
       </c>
     </row>
@@ -6182,7 +6182,7 @@
         <v>2020</v>
       </c>
       <c r="D63" t="n">
-        <v>17227</v>
+        <v>17199</v>
       </c>
       <c r="E63" t="n">
         <v>16041</v>
@@ -6218,13 +6218,13 @@
         <v>15928.4</v>
       </c>
       <c r="P63" t="n">
-        <v>1691.6</v>
+        <v>1663.6</v>
       </c>
       <c r="Q63" t="n">
         <v>393</v>
       </c>
       <c r="R63" t="n">
-        <v>10.9</v>
+        <v>10.7</v>
       </c>
       <c r="S63" t="n">
         <v>2.7</v>
@@ -6236,26 +6236,26 @@
       </c>
       <c r="U63" t="inlineStr">
         <is>
-          <t>1691.6 (±393.0)</t>
+          <t>1663.6 (±393.0)</t>
         </is>
       </c>
       <c r="V63" t="inlineStr">
         <is>
-          <t>10.9% (±2.7%)</t>
+          <t>10.7% (±2.7%)</t>
         </is>
       </c>
       <c r="W63" t="n">
         <v>3674887</v>
       </c>
       <c r="X63" t="n">
-        <v>46</v>
+        <v>45.3</v>
       </c>
       <c r="Y63" t="n">
         <v>10.7</v>
       </c>
       <c r="Z63" t="inlineStr">
         <is>
-          <t>46.0(±10.7)</t>
+          <t>45.3(±10.7)</t>
         </is>
       </c>
     </row>
@@ -6366,7 +6366,7 @@
         <v>2020</v>
       </c>
       <c r="D65" t="n">
-        <v>42708</v>
+        <v>42709</v>
       </c>
       <c r="E65" t="n">
         <v>38306</v>
@@ -6402,7 +6402,7 @@
         <v>38641.69999999999</v>
       </c>
       <c r="P65" t="n">
-        <v>4556.4</v>
+        <v>4557.4</v>
       </c>
       <c r="Q65" t="n">
         <v>490.1</v>
@@ -6420,7 +6420,7 @@
       </c>
       <c r="U65" t="inlineStr">
         <is>
-          <t>4556.4 (±490.1)</t>
+          <t>4557.4 (±490.1)</t>
         </is>
       </c>
       <c r="V65" t="inlineStr">
@@ -6550,7 +6550,7 @@
         <v>2020</v>
       </c>
       <c r="D67" t="n">
-        <v>5243</v>
+        <v>5245</v>
       </c>
       <c r="E67" t="n">
         <v>5059</v>
@@ -6586,7 +6586,7 @@
         <v>5054.9</v>
       </c>
       <c r="P67" t="n">
-        <v>305.2</v>
+        <v>307.2</v>
       </c>
       <c r="Q67" t="n">
         <v>117.1</v>
@@ -6595,7 +6595,7 @@
         <v>6.2</v>
       </c>
       <c r="S67" t="n">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="T67" t="inlineStr">
         <is>
@@ -6604,26 +6604,26 @@
       </c>
       <c r="U67" t="inlineStr">
         <is>
-          <t>305.2 (±117.1)</t>
+          <t>307.2 (±117.1)</t>
         </is>
       </c>
       <c r="V67" t="inlineStr">
         <is>
-          <t>6.2% (±2.5%)</t>
+          <t>6.2% (±2.4%)</t>
         </is>
       </c>
       <c r="W67" t="n">
         <v>1202898</v>
       </c>
       <c r="X67" t="n">
-        <v>25.4</v>
+        <v>25.5</v>
       </c>
       <c r="Y67" t="n">
-        <v>9.699999999999999</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="Z67" t="inlineStr">
         <is>
-          <t>25.4(±9.7)</t>
+          <t>25.5(±9.8)</t>
         </is>
       </c>
     </row>
@@ -6642,7 +6642,7 @@
         <v>2020</v>
       </c>
       <c r="D68" t="n">
-        <v>15254</v>
+        <v>15255</v>
       </c>
       <c r="E68" t="n">
         <v>14750</v>
@@ -6678,7 +6678,7 @@
         <v>15043</v>
       </c>
       <c r="P68" t="n">
-        <v>303.2</v>
+        <v>304.2</v>
       </c>
       <c r="Q68" t="n">
         <v>92.2</v>
@@ -6696,7 +6696,7 @@
       </c>
       <c r="U68" t="inlineStr">
         <is>
-          <t>303.2 (±92.2)</t>
+          <t>304.2 (±92.2)</t>
         </is>
       </c>
       <c r="V68" t="inlineStr">
@@ -6734,7 +6734,7 @@
         <v>2020</v>
       </c>
       <c r="D69" t="n">
-        <v>167992</v>
+        <v>168035</v>
       </c>
       <c r="E69" t="n">
         <v>152008</v>
@@ -6770,16 +6770,16 @@
         <v>155840.2</v>
       </c>
       <c r="P69" t="n">
-        <v>12771</v>
+        <v>12814</v>
       </c>
       <c r="Q69" t="n">
         <v>619.2</v>
       </c>
       <c r="R69" t="n">
-        <v>8.199999999999999</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="S69" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="T69" t="inlineStr">
         <is>
@@ -6788,12 +6788,12 @@
       </c>
       <c r="U69" t="inlineStr">
         <is>
-          <t>12771.0 (±619.2)</t>
+          <t>12814.0 (±619.2)</t>
         </is>
       </c>
       <c r="V69" t="inlineStr">
         <is>
-          <t>8.2% (±0.4%)</t>
+          <t>8.3% (±0.5%)</t>
         </is>
       </c>
       <c r="W69" t="n">
@@ -7102,7 +7102,7 @@
         <v>2020</v>
       </c>
       <c r="D73" t="n">
-        <v>149547</v>
+        <v>149569</v>
       </c>
       <c r="E73" t="n">
         <v>133789</v>
@@ -7138,7 +7138,7 @@
         <v>133179.6</v>
       </c>
       <c r="P73" t="n">
-        <v>19583.2</v>
+        <v>19605.2</v>
       </c>
       <c r="Q73" t="n">
         <v>3215.8</v>
@@ -7156,7 +7156,7 @@
       </c>
       <c r="U73" t="inlineStr">
         <is>
-          <t>19583.2 (±3215.8)</t>
+          <t>19605.2 (±3215.8)</t>
         </is>
       </c>
       <c r="V73" t="inlineStr">
@@ -7168,14 +7168,14 @@
         <v>52577772</v>
       </c>
       <c r="X73" t="n">
-        <v>37.2</v>
+        <v>37.3</v>
       </c>
       <c r="Y73" t="n">
-        <v>6.2</v>
+        <v>6.1</v>
       </c>
       <c r="Z73" t="inlineStr">
         <is>
-          <t>37.2(±6.2)</t>
+          <t>37.3(±6.1)</t>
         </is>
       </c>
     </row>
@@ -7286,7 +7286,7 @@
         <v>2020</v>
       </c>
       <c r="D75" t="n">
-        <v>15175</v>
+        <v>15463</v>
       </c>
       <c r="E75" t="n">
         <v>15142</v>
@@ -7322,16 +7322,16 @@
         <v>14728.5</v>
       </c>
       <c r="P75" t="n">
-        <v>1317.8</v>
+        <v>1605.8</v>
       </c>
       <c r="Q75" t="n">
         <v>871.3</v>
       </c>
       <c r="R75" t="n">
-        <v>9.5</v>
+        <v>11.6</v>
       </c>
       <c r="S75" t="n">
-        <v>6.5</v>
+        <v>6.6</v>
       </c>
       <c r="T75" t="inlineStr">
         <is>
@@ -7340,26 +7340,26 @@
       </c>
       <c r="U75" t="inlineStr">
         <is>
-          <t>1317.8 (±871.3)</t>
+          <t>1605.8 (±871.3)</t>
         </is>
       </c>
       <c r="V75" t="inlineStr">
         <is>
-          <t>9.5% (±6.5%)</t>
+          <t>11.6% (±6.6%)</t>
         </is>
       </c>
       <c r="W75" t="n">
         <v>2519134</v>
       </c>
       <c r="X75" t="n">
-        <v>52.3</v>
+        <v>63.7</v>
       </c>
       <c r="Y75" t="n">
         <v>34.6</v>
       </c>
       <c r="Z75" t="inlineStr">
         <is>
-          <t>52.3(±34.6)</t>
+          <t>63.7(±34.6)</t>
         </is>
       </c>
     </row>
@@ -7378,7 +7378,7 @@
         <v>2020</v>
       </c>
       <c r="D76" t="n">
-        <v>1326</v>
+        <v>1292</v>
       </c>
       <c r="E76" t="n">
         <v>1089</v>
@@ -7414,16 +7414,16 @@
         <v>1225</v>
       </c>
       <c r="P76" t="n">
-        <v>146.2</v>
+        <v>112.2</v>
       </c>
       <c r="Q76" t="n">
         <v>45.2</v>
       </c>
       <c r="R76" t="n">
-        <v>12.4</v>
+        <v>9.5</v>
       </c>
       <c r="S76" t="n">
-        <v>4.2</v>
+        <v>4</v>
       </c>
       <c r="T76" t="inlineStr">
         <is>
@@ -7432,26 +7432,26 @@
       </c>
       <c r="U76" t="inlineStr">
         <is>
-          <t>146.2 (±45.2)</t>
+          <t>112.2 (±45.2)</t>
         </is>
       </c>
       <c r="V76" t="inlineStr">
         <is>
-          <t>12.4% (±4.2%)</t>
+          <t>9.5% (±4.0%)</t>
         </is>
       </c>
       <c r="W76" t="n">
         <v>584891</v>
       </c>
       <c r="X76" t="n">
-        <v>25</v>
+        <v>19.2</v>
       </c>
       <c r="Y76" t="n">
         <v>7.7</v>
       </c>
       <c r="Z76" t="inlineStr">
         <is>
-          <t>25.0(±7.7)</t>
+          <t>19.2(±7.7)</t>
         </is>
       </c>
     </row>
@@ -7562,7 +7562,7 @@
         <v>2020</v>
       </c>
       <c r="D78" t="n">
-        <v>2768</v>
+        <v>2799</v>
       </c>
       <c r="E78" t="n">
         <v>2284</v>
@@ -7598,13 +7598,13 @@
         <v>2383.5</v>
       </c>
       <c r="P78" t="n">
-        <v>432.4</v>
+        <v>463.4</v>
       </c>
       <c r="Q78" t="n">
         <v>47.9</v>
       </c>
       <c r="R78" t="n">
-        <v>18.5</v>
+        <v>19.8</v>
       </c>
       <c r="S78" t="n">
         <v>2.4</v>
@@ -7616,26 +7616,26 @@
       </c>
       <c r="U78" t="inlineStr">
         <is>
-          <t>432.4 (±47.9)</t>
+          <t>463.4 (±47.9)</t>
         </is>
       </c>
       <c r="V78" t="inlineStr">
         <is>
-          <t>18.5% (±2.4%)</t>
+          <t>19.8% (±2.4%)</t>
         </is>
       </c>
       <c r="W78" t="n">
         <v>584830</v>
       </c>
       <c r="X78" t="n">
-        <v>73.90000000000001</v>
+        <v>79.2</v>
       </c>
       <c r="Y78" t="n">
         <v>8.199999999999999</v>
       </c>
       <c r="Z78" t="inlineStr">
         <is>
-          <t>73.9(±8.2)</t>
+          <t>79.2(±8.2)</t>
         </is>
       </c>
     </row>
@@ -7746,7 +7746,7 @@
         <v>2020</v>
       </c>
       <c r="D80" t="n">
-        <v>10296</v>
+        <v>10297</v>
       </c>
       <c r="E80" t="n">
         <v>10356</v>
@@ -7782,7 +7782,7 @@
         <v>10516.4</v>
       </c>
       <c r="P80" t="n">
-        <v>-163.6</v>
+        <v>-162.6</v>
       </c>
       <c r="Q80" t="n">
         <v>56.8</v>
@@ -7800,7 +7800,7 @@
       </c>
       <c r="U80" t="inlineStr">
         <is>
-          <t>-163.6 (±56.8)</t>
+          <t>-162.6 (±56.8)</t>
         </is>
       </c>
       <c r="V80" t="inlineStr">
@@ -7815,11 +7815,11 @@
         <v>-3.3</v>
       </c>
       <c r="Y80" t="n">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
       <c r="Z80" t="inlineStr">
         <is>
-          <t>-3.3(±1.1)</t>
+          <t>-3.3(±1.2)</t>
         </is>
       </c>
     </row>
@@ -7930,7 +7930,7 @@
         <v>2020</v>
       </c>
       <c r="D82" t="n">
-        <v>28934</v>
+        <v>29040</v>
       </c>
       <c r="E82" t="n">
         <v>25842</v>
@@ -7966,13 +7966,13 @@
         <v>26768.00000000001</v>
       </c>
       <c r="P82" t="n">
-        <v>2338.2</v>
+        <v>2444.2</v>
       </c>
       <c r="Q82" t="n">
         <v>172.2</v>
       </c>
       <c r="R82" t="n">
-        <v>8.800000000000001</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="S82" t="n">
         <v>0.7</v>
@@ -7984,26 +7984,26 @@
       </c>
       <c r="U82" t="inlineStr">
         <is>
-          <t>2338.2 (±172.2)</t>
+          <t>2444.2 (±172.2)</t>
         </is>
       </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>8.8% (±0.7%)</t>
+          <t>9.2% (±0.7%)</t>
         </is>
       </c>
       <c r="W82" t="n">
         <v>9187988</v>
       </c>
       <c r="X82" t="n">
-        <v>25.4</v>
+        <v>26.6</v>
       </c>
       <c r="Y82" t="n">
         <v>1.9</v>
       </c>
       <c r="Z82" t="inlineStr">
         <is>
-          <t>25.4(±1.9)</t>
+          <t>26.6(±1.9)</t>
         </is>
       </c>
     </row>
@@ -8114,7 +8114,7 @@
         <v>2020</v>
       </c>
       <c r="D84" t="n">
-        <v>23310</v>
+        <v>23303</v>
       </c>
       <c r="E84" t="n">
         <v>20936</v>
@@ -8150,16 +8150,16 @@
         <v>21169.3</v>
       </c>
       <c r="P84" t="n">
-        <v>2362.2</v>
+        <v>2355.2</v>
       </c>
       <c r="Q84" t="n">
         <v>221.5</v>
       </c>
       <c r="R84" t="n">
-        <v>11.3</v>
+        <v>11.2</v>
       </c>
       <c r="S84" t="n">
-        <v>1.2</v>
+        <v>1.1</v>
       </c>
       <c r="T84" t="inlineStr">
         <is>
@@ -8168,26 +8168,26 @@
       </c>
       <c r="U84" t="inlineStr">
         <is>
-          <t>2362.2 (±221.5)</t>
+          <t>2355.2 (±221.5)</t>
         </is>
       </c>
       <c r="V84" t="inlineStr">
         <is>
-          <t>11.3% (±1.2%)</t>
+          <t>11.2% (±1.1%)</t>
         </is>
       </c>
       <c r="W84" t="n">
         <v>5113344</v>
       </c>
       <c r="X84" t="n">
-        <v>46.2</v>
+        <v>46.1</v>
       </c>
       <c r="Y84" t="n">
         <v>4.3</v>
       </c>
       <c r="Z84" t="inlineStr">
         <is>
-          <t>46.2(±4.3)</t>
+          <t>46.1(±4.3)</t>
         </is>
       </c>
     </row>
@@ -8298,7 +8298,7 @@
         <v>2020</v>
       </c>
       <c r="D86" t="n">
-        <v>110413</v>
+        <v>110418</v>
       </c>
       <c r="E86" t="n">
         <v>92883</v>
@@ -8334,7 +8334,7 @@
         <v>94541.90000000001</v>
       </c>
       <c r="P86" t="n">
-        <v>16310.2</v>
+        <v>16315.2</v>
       </c>
       <c r="Q86" t="n">
         <v>439.1</v>
@@ -8352,7 +8352,7 @@
       </c>
       <c r="U86" t="inlineStr">
         <is>
-          <t>16310.2 (±439.1)</t>
+          <t>16315.2 (±439.1)</t>
         </is>
       </c>
       <c r="V86" t="inlineStr">
@@ -8482,7 +8482,7 @@
         <v>2020</v>
       </c>
       <c r="D88" t="n">
-        <v>15831</v>
+        <v>15859</v>
       </c>
       <c r="E88" t="n">
         <v>15637</v>
@@ -8518,13 +8518,13 @@
         <v>15574.2</v>
       </c>
       <c r="P88" t="n">
-        <v>539.6</v>
+        <v>567.6</v>
       </c>
       <c r="Q88" t="n">
         <v>282.8</v>
       </c>
       <c r="R88" t="n">
-        <v>3.5</v>
+        <v>3.7</v>
       </c>
       <c r="S88" t="n">
         <v>1.9</v>
@@ -8536,26 +8536,26 @@
       </c>
       <c r="U88" t="inlineStr">
         <is>
-          <t>539.6 (±282.8)</t>
+          <t>567.6 (±282.8)</t>
         </is>
       </c>
       <c r="V88" t="inlineStr">
         <is>
-          <t>3.5% (±1.9%)</t>
+          <t>3.7% (±1.9%)</t>
         </is>
       </c>
       <c r="W88" t="n">
         <v>7830936</v>
       </c>
       <c r="X88" t="n">
-        <v>6.9</v>
+        <v>7.2</v>
       </c>
       <c r="Y88" t="n">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="Z88" t="inlineStr">
         <is>
-          <t>6.9(±3.6)</t>
+          <t>7.2(±3.7)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added more comments. Added suppressors for Webdriver Manager logging, and warning catcher and silencer for a OpenPYXL warning about file style.
Signed-off-by: Mlad-en <mmladenov1992@gmail.com>
</commit_message>
<xml_diff>
--- a/data_output/Excess Mortality/Countries/TOTAL_EUROPE_(0-4) - (70-74)_['Female', 'Male', 'Total']_excess_mortality_2020.xlsx
+++ b/data_output/Excess Mortality/Countries/TOTAL_EUROPE_(0-4) - (70-74)_['Female', 'Male', 'Total']_excess_mortality_2020.xlsx
@@ -1030,7 +1030,7 @@
         <v>2020</v>
       </c>
       <c r="D7" t="n">
-        <v>14819</v>
+        <v>14822</v>
       </c>
       <c r="E7" t="n">
         <v>13428</v>
@@ -1066,7 +1066,7 @@
         <v>13589.2</v>
       </c>
       <c r="P7" t="n">
-        <v>1415</v>
+        <v>1418</v>
       </c>
       <c r="Q7" t="n">
         <v>185.2</v>
@@ -1075,7 +1075,7 @@
         <v>10.6</v>
       </c>
       <c r="S7" t="n">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="T7" t="inlineStr">
         <is>
@@ -1084,26 +1084,26 @@
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>1415.0 (±185.2)</t>
+          <t>1418.0 (±185.2)</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>10.6% (±1.6%)</t>
+          <t>10.6% (±1.5%)</t>
         </is>
       </c>
       <c r="W7" t="n">
         <v>4888989</v>
       </c>
       <c r="X7" t="n">
-        <v>28.9</v>
+        <v>29</v>
       </c>
       <c r="Y7" t="n">
         <v>3.8</v>
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>28.9(±3.8)</t>
+          <t>29.0(±3.8)</t>
         </is>
       </c>
     </row>
@@ -1674,7 +1674,7 @@
         <v>2020</v>
       </c>
       <c r="D14" t="n">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E14" t="n">
         <v>249</v>
@@ -1710,13 +1710,13 @@
         <v>255.6000000000001</v>
       </c>
       <c r="P14" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q14" t="n">
         <v>14.6</v>
       </c>
       <c r="R14" t="n">
-        <v>4.6</v>
+        <v>5</v>
       </c>
       <c r="S14" t="n">
         <v>6</v>
@@ -1728,26 +1728,26 @@
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>11.0 (±14.6)</t>
+          <t>12.0 (±14.6)</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>4.6% (±6.0%)</t>
+          <t>5.0% (±6.0%)</t>
         </is>
       </c>
       <c r="W14" t="n">
         <v>165097</v>
       </c>
       <c r="X14" t="n">
-        <v>6.7</v>
+        <v>7.3</v>
       </c>
       <c r="Y14" t="n">
         <v>8.800000000000001</v>
       </c>
       <c r="Z14" t="inlineStr">
         <is>
-          <t>6.7(±8.8)</t>
+          <t>7.3(±8.8)</t>
         </is>
       </c>
     </row>
@@ -3698,7 +3698,7 @@
         <v>2020</v>
       </c>
       <c r="D36" t="n">
-        <v>27890</v>
+        <v>27891</v>
       </c>
       <c r="E36" t="n">
         <v>24878</v>
@@ -3734,7 +3734,7 @@
         <v>25057.5</v>
       </c>
       <c r="P36" t="n">
-        <v>3142.4</v>
+        <v>3143.4</v>
       </c>
       <c r="Q36" t="n">
         <v>309.9</v>
@@ -3752,7 +3752,7 @@
       </c>
       <c r="U36" t="inlineStr">
         <is>
-          <t>3142.4 (±309.9)</t>
+          <t>3143.4 (±309.9)</t>
         </is>
       </c>
       <c r="V36" t="inlineStr">
@@ -3882,7 +3882,7 @@
         <v>2020</v>
       </c>
       <c r="D38" t="n">
-        <v>3501</v>
+        <v>3502</v>
       </c>
       <c r="E38" t="n">
         <v>3415</v>
@@ -3918,13 +3918,13 @@
         <v>3414.2</v>
       </c>
       <c r="P38" t="n">
-        <v>161.4</v>
+        <v>162.4</v>
       </c>
       <c r="Q38" t="n">
         <v>74.59999999999999</v>
       </c>
       <c r="R38" t="n">
-        <v>4.8</v>
+        <v>4.9</v>
       </c>
       <c r="S38" t="n">
         <v>2.3</v>
@@ -3936,26 +3936,26 @@
       </c>
       <c r="U38" t="inlineStr">
         <is>
-          <t>161.4 (±74.6)</t>
+          <t>162.4 (±74.6)</t>
         </is>
       </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>4.8% (±2.3%)</t>
+          <t>4.9% (±2.3%)</t>
         </is>
       </c>
       <c r="W38" t="n">
         <v>592881</v>
       </c>
       <c r="X38" t="n">
-        <v>27.2</v>
+        <v>27.4</v>
       </c>
       <c r="Y38" t="n">
         <v>12.6</v>
       </c>
       <c r="Z38" t="inlineStr">
         <is>
-          <t>27.2(±12.6)</t>
+          <t>27.4(±12.6)</t>
         </is>
       </c>
     </row>
@@ -4342,7 +4342,7 @@
         <v>2020</v>
       </c>
       <c r="D43" t="n">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="E43" t="n">
         <v>340</v>
@@ -4378,16 +4378,16 @@
         <v>393.6000000000001</v>
       </c>
       <c r="P43" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="Q43" t="n">
         <v>14.6</v>
       </c>
       <c r="R43" t="n">
-        <v>1.8</v>
+        <v>2.9</v>
       </c>
       <c r="S43" t="n">
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
       <c r="T43" t="inlineStr">
         <is>
@@ -4396,26 +4396,26 @@
       </c>
       <c r="U43" t="inlineStr">
         <is>
-          <t>7.0 (±14.6)</t>
+          <t>11.0 (±14.6)</t>
         </is>
       </c>
       <c r="V43" t="inlineStr">
         <is>
-          <t>1.8% (±3.7%)</t>
+          <t>2.9% (±3.8%)</t>
         </is>
       </c>
       <c r="W43" t="n">
         <v>177162</v>
       </c>
       <c r="X43" t="n">
-        <v>4</v>
+        <v>6.2</v>
       </c>
       <c r="Y43" t="n">
-        <v>8.199999999999999</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="Z43" t="inlineStr">
         <is>
-          <t>4.0(±8.2)</t>
+          <t>6.2(±8.3)</t>
         </is>
       </c>
     </row>
@@ -6366,7 +6366,7 @@
         <v>2020</v>
       </c>
       <c r="D65" t="n">
-        <v>42709</v>
+        <v>42713</v>
       </c>
       <c r="E65" t="n">
         <v>38306</v>
@@ -6402,16 +6402,16 @@
         <v>38641.69999999999</v>
       </c>
       <c r="P65" t="n">
-        <v>4557.4</v>
+        <v>4561.4</v>
       </c>
       <c r="Q65" t="n">
         <v>490.1</v>
       </c>
       <c r="R65" t="n">
-        <v>11.9</v>
+        <v>12</v>
       </c>
       <c r="S65" t="n">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="T65" t="inlineStr">
         <is>
@@ -6420,12 +6420,12 @@
       </c>
       <c r="U65" t="inlineStr">
         <is>
-          <t>4557.4 (±490.1)</t>
+          <t>4561.4 (±490.1)</t>
         </is>
       </c>
       <c r="V65" t="inlineStr">
         <is>
-          <t>11.9% (±1.4%)</t>
+          <t>12.0% (±1.5%)</t>
         </is>
       </c>
       <c r="W65" t="n">
@@ -6550,7 +6550,7 @@
         <v>2020</v>
       </c>
       <c r="D67" t="n">
-        <v>5245</v>
+        <v>5246</v>
       </c>
       <c r="E67" t="n">
         <v>5059</v>
@@ -6586,7 +6586,7 @@
         <v>5054.9</v>
       </c>
       <c r="P67" t="n">
-        <v>307.2</v>
+        <v>308.2</v>
       </c>
       <c r="Q67" t="n">
         <v>117.1</v>
@@ -6604,7 +6604,7 @@
       </c>
       <c r="U67" t="inlineStr">
         <is>
-          <t>307.2 (±117.1)</t>
+          <t>308.2 (±117.1)</t>
         </is>
       </c>
       <c r="V67" t="inlineStr">
@@ -6616,14 +6616,14 @@
         <v>1202898</v>
       </c>
       <c r="X67" t="n">
-        <v>25.5</v>
+        <v>25.6</v>
       </c>
       <c r="Y67" t="n">
         <v>9.800000000000001</v>
       </c>
       <c r="Z67" t="inlineStr">
         <is>
-          <t>25.5(±9.8)</t>
+          <t>25.6(±9.8)</t>
         </is>
       </c>
     </row>
@@ -7010,7 +7010,7 @@
         <v>2020</v>
       </c>
       <c r="D72" t="n">
-        <v>638</v>
+        <v>643</v>
       </c>
       <c r="E72" t="n">
         <v>589</v>
@@ -7046,13 +7046,13 @@
         <v>633.5999999999999</v>
       </c>
       <c r="P72" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="Q72" t="n">
         <v>13.6</v>
       </c>
       <c r="R72" t="n">
-        <v>2.9</v>
+        <v>3.7</v>
       </c>
       <c r="S72" t="n">
         <v>2.2</v>
@@ -7064,26 +7064,26 @@
       </c>
       <c r="U72" t="inlineStr">
         <is>
-          <t>18.0 (±13.6)</t>
+          <t>23.0 (±13.6)</t>
         </is>
       </c>
       <c r="V72" t="inlineStr">
         <is>
-          <t>2.9% (±2.2%)</t>
+          <t>3.7% (±2.2%)</t>
         </is>
       </c>
       <c r="W72" t="n">
         <v>342259</v>
       </c>
       <c r="X72" t="n">
-        <v>5.3</v>
+        <v>6.7</v>
       </c>
       <c r="Y72" t="n">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="Z72" t="inlineStr">
         <is>
-          <t>5.3(±3.9)</t>
+          <t>6.7(±4.0)</t>
         </is>
       </c>
     </row>

</xml_diff>